<commit_message>
database fixes and added thesisProposal fields
</commit_message>
<xml_diff>
--- a/database/proposalKeyWords.xlsx
+++ b/database/proposalKeyWords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisa\OneDrive\Desktop\diana\adding thesis\ThesisManagement-Group09\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\Desktop\POLI magy\Software Engineering 2\main project\ThesisManagement-Group09\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27265839-A325-4F63-917F-7FA2D5E97BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7126738F-46F8-486E-94B8-42F3CFC6D0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6096" yWindow="2868" windowWidth="15120" windowHeight="8304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>chemistry</t>
+    <t>AI</t>
   </si>
   <si>
-    <t>sustainable</t>
+    <t>web development</t>
   </si>
   <si>
-    <t>fibers</t>
+    <t>research</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>